<commit_message>
पशु valuation given anjan sharma complete kurthali truss valuation given kurthali sadak printed school rastriya maa bi. remained
</commit_message>
<xml_diff>
--- a/ofc/estimates/new track bheterinary ukhutaar sadak/V anjan sharma.xlsx
+++ b/ofc/estimates/new track bheterinary ukhutaar sadak/V anjan sharma.xlsx
@@ -2,29 +2,31 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\new track bheterinary ukhutaar sadak\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\081-082\ofc\ofc\estimates\new track bheterinary ukhutaar sadak\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="estimate" sheetId="18" r:id="rId1"/>
     <sheet name="WCR" sheetId="6" r:id="rId2"/>
     <sheet name="V" sheetId="19" r:id="rId3"/>
+    <sheet name="M" sheetId="20" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="description_103">[1]Abstract!$B$16</definedName>
     <definedName name="description_124" localSheetId="0">#REF!</definedName>
+    <definedName name="description_124" localSheetId="3">#REF!</definedName>
     <definedName name="description_124" localSheetId="2">#REF!</definedName>
     <definedName name="description_124">#REF!</definedName>
     <definedName name="description_247">[1]Abstract!$B$22</definedName>
@@ -39,12 +41,14 @@
     <definedName name="description_759">[1]Abstract!$B$278</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">estimate!$A$1:$K$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">M!$A$1:$K$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">V!$A$1:$K$44</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">estimate!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">M!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">V!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="52">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -187,9 +191,6 @@
     <t>F.Y.: 2081/2082</t>
   </si>
   <si>
-    <t>sqm</t>
-  </si>
-  <si>
     <t>Earthwork Excavation in Cutting., Roadway Excavation in all types of Soil by Mechanical  Means ., Road way Excavation in  all types of soil as per Drawing and technical specifications  including  removal of stumps and other deleterious matter, all lifts and lead as per Drawing and instruction of the Engineer.</t>
   </si>
   <si>
@@ -205,9 +206,6 @@
     <t>Total Valuated</t>
   </si>
   <si>
-    <t>Date:2082/03/01</t>
-  </si>
-  <si>
     <t>-drain</t>
   </si>
   <si>
@@ -219,14 +217,20 @@
   <si>
     <t xml:space="preserve">Date:                  </t>
   </si>
+  <si>
+    <t>Detail Quantity Measurement Sheet</t>
+  </si>
+  <si>
+    <t>cum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -398,9 +402,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -408,7 +412,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -428,14 +432,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -444,7 +448,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,7 +473,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -501,7 +505,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -509,7 +513,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -524,7 +528,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -540,7 +544,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -554,22 +558,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -584,6 +576,39 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -605,21 +630,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1179,134 +1191,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-    </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+    </row>
+    <row r="2" spans="1:30" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-    </row>
-    <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-    </row>
-    <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+    </row>
+    <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+    </row>
+    <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-    </row>
-    <row r="5" spans="1:30" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="s">
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+    </row>
+    <row r="5" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-    </row>
-    <row r="6" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+    </row>
+    <row r="6" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="69" t="s">
+      <c r="H6" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-    </row>
-    <row r="7" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="75" t="s">
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+    </row>
+    <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="76" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
-    </row>
-    <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+    </row>
+    <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1341,12 +1353,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>1</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="38"/>
@@ -1365,10 +1377,10 @@
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
     </row>
-    <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="36">
         <v>1</v>
@@ -1409,7 +1421,7 @@
       <c r="AC10" s="48"/>
       <c r="AD10" s="48"/>
     </row>
-    <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
         <v>39</v>
@@ -1423,7 +1435,7 @@
         <v>720</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="I11" s="40">
         <v>64.63</v>
@@ -1452,7 +1464,7 @@
       <c r="AC11" s="48"/>
       <c r="AD11" s="48"/>
     </row>
-    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
         <v>38</v>
@@ -1477,7 +1489,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="37"/>
       <c r="C13" s="42"/>
@@ -1490,7 +1502,7 @@
       <c r="J13" s="44"/>
       <c r="K13" s="36"/>
     </row>
-    <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -1526,7 +1538,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="24"/>
       <c r="C15" s="19"/>
@@ -1546,7 +1558,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
       <c r="B16" s="45" t="s">
         <v>17</v>
@@ -1564,7 +1576,7 @@
       </c>
       <c r="K16" s="36"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="57"/>
       <c r="B17" s="60"/>
       <c r="C17" s="61"/>
@@ -1577,16 +1589,16 @@
       <c r="J17" s="59"/>
       <c r="K17" s="56"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
       <c r="B18" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="74">
+      <c r="C18" s="70">
         <f>J16</f>
         <v>52047.44</v>
       </c>
-      <c r="D18" s="74"/>
+      <c r="D18" s="70"/>
       <c r="E18" s="51"/>
       <c r="F18" s="50"/>
       <c r="G18" s="51"/>
@@ -1595,15 +1607,15 @@
       <c r="J18" s="53"/>
       <c r="K18" s="54"/>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="55"/>
       <c r="B19" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="77">
+      <c r="C19" s="73">
         <v>40000</v>
       </c>
-      <c r="D19" s="77"/>
+      <c r="D19" s="73"/>
       <c r="E19" s="67"/>
       <c r="F19" s="48"/>
       <c r="G19" s="47"/>
@@ -1612,16 +1624,16 @@
       <c r="J19" s="47"/>
       <c r="K19" s="48"/>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="55"/>
       <c r="B20" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="78">
+      <c r="C20" s="74">
         <f>C19-C22-C23</f>
         <v>38000</v>
       </c>
-      <c r="D20" s="78"/>
+      <c r="D20" s="74"/>
       <c r="E20" s="39">
         <f>C20/C18*100</f>
         <v>73.010315204743975</v>
@@ -1633,16 +1645,16 @@
       <c r="J20" s="47"/>
       <c r="K20" s="48"/>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="55"/>
       <c r="B21" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="74">
+      <c r="C21" s="70">
         <f>C18-C20</f>
         <v>14047.440000000002</v>
       </c>
-      <c r="D21" s="74"/>
+      <c r="D21" s="70"/>
       <c r="E21" s="39">
         <f>100-E20</f>
         <v>26.989684795256025</v>
@@ -1654,16 +1666,16 @@
       <c r="J21" s="47"/>
       <c r="K21" s="48"/>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="55"/>
       <c r="B22" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="74">
+      <c r="C22" s="70">
         <f>C19*0.03</f>
         <v>1200</v>
       </c>
-      <c r="D22" s="74"/>
+      <c r="D22" s="70"/>
       <c r="E22" s="39">
         <v>3</v>
       </c>
@@ -1674,16 +1686,16 @@
       <c r="J22" s="47"/>
       <c r="K22" s="48"/>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="55"/>
       <c r="B23" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="74">
+      <c r="C23" s="70">
         <f>C19*0.02</f>
         <v>800</v>
       </c>
-      <c r="D23" s="74"/>
+      <c r="D23" s="70"/>
       <c r="E23" s="39">
         <v>2</v>
       </c>
@@ -1694,7 +1706,7 @@
       <c r="J23" s="47"/>
       <c r="K23" s="48"/>
     </row>
-    <row r="24" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="56"/>
       <c r="B24" s="56"/>
       <c r="C24" s="56"/>
@@ -1707,62 +1719,69 @@
       <c r="J24" s="56"/>
       <c r="K24" s="56"/>
     </row>
-    <row r="25" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="33" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="38" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="39" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="40" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="43" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="A7:F7"/>
@@ -1771,21 +1790,11 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;LPrepared By:
-Kristal Suwal&amp;CChecked By:
-Er. Milan Phuyal&amp;RApproved By:
-Er. Prakash Singh Saud</oddFooter>
+    <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1794,110 +1803,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="89" t="s">
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="90" t="s">
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="86">
+      <c r="C6" s="81">
         <f>F18</f>
         <v>52047.44</v>
       </c>
-      <c r="D6" s="87"/>
+      <c r="D6" s="82"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1905,90 +1914,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="86">
+      <c r="J6" s="81">
         <f>I18</f>
-        <v>45495.768891083135</v>
-      </c>
-      <c r="K6" s="87"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45859.106749416474</v>
+      </c>
+      <c r="K6" s="82"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="I7" s="82" t="s">
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="I7" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="68" t="str">
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="75" t="str">
         <f>estimate!A6</f>
         <v>Project:- ६. नं. कृषि सडक</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="I8" s="83" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="84" t="str">
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="I8" s="90" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="91" t="str">
         <f>estimate!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="I9" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="79" t="s">
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="I9" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="85" t="s">
+      <c r="D11" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85" t="s">
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="79" t="s">
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="80" t="s">
+      <c r="K11" s="87" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="79"/>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="86"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2007,10 +2016,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="79"/>
-      <c r="K12" s="80"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="J12" s="86"/>
+      <c r="K12" s="87"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <f>estimate!A9</f>
         <v>1</v>
@@ -2021,7 +2030,7 @@
       </c>
       <c r="C13" s="12" t="str">
         <f>estimate!H11</f>
-        <v>sqm</v>
+        <v>cum</v>
       </c>
       <c r="D13" s="12">
         <f>estimate!G11</f>
@@ -2037,7 +2046,7 @@
       </c>
       <c r="G13" s="12">
         <f>V!G32</f>
-        <v>635.47197691252677</v>
+        <v>640.54697691252682</v>
       </c>
       <c r="H13" s="12">
         <f>V!I32</f>
@@ -2045,15 +2054,15 @@
       </c>
       <c r="I13" s="12">
         <f>G13*H13</f>
-        <v>41070.553867856601</v>
+        <v>41398.551117856608</v>
       </c>
       <c r="J13" s="28">
         <f>I13-F13</f>
-        <v>-5463.0461321433977</v>
+        <v>-5135.0488821433901</v>
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="33" t="str">
         <f>estimate!B12</f>
@@ -2070,12 +2079,12 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12">
         <f>V!J33</f>
-        <v>4425.2150232265321</v>
+        <v>4460.555631559866</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="12"/>
@@ -2088,7 +2097,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <f>estimate!A14</f>
         <v>2</v>
@@ -2131,7 +2140,7 @@
       </c>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="12"/>
@@ -2144,7 +2153,7 @@
       <c r="J17" s="28"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
@@ -2160,23 +2169,16 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7">
         <f>SUM(I13:I16)</f>
-        <v>45495.768891083135</v>
+        <v>45859.106749416474</v>
       </c>
       <c r="J18" s="13">
         <f>I18-F18</f>
-        <v>-6551.6711089168675</v>
+        <v>-6188.3332505835278</v>
       </c>
       <c r="K18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2190,6 +2192,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2207,134 +2216,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:K7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-    </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-    </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-    </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+    </row>
+    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+    </row>
+    <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-    </row>
-    <row r="5" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-    </row>
-    <row r="6" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+    </row>
+    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="69" t="s">
+      <c r="H6" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-    </row>
-    <row r="7" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="75" t="s">
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="76" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
-    </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -2369,12 +2378,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>1</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="38"/>
@@ -2395,10 +2404,10 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="36">
         <v>0.5</v>
@@ -2439,7 +2448,7 @@
       <c r="T10" s="48"/>
       <c r="U10" s="48"/>
     </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="37"/>
       <c r="C11" s="36">
@@ -2481,7 +2490,7 @@
       <c r="T11" s="48"/>
       <c r="U11" s="48"/>
     </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="37"/>
       <c r="C12" s="36">
@@ -2524,7 +2533,7 @@
       <c r="T12" s="48"/>
       <c r="U12" s="48"/>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="37"/>
       <c r="C13" s="36">
@@ -2567,7 +2576,7 @@
       <c r="T13" s="48"/>
       <c r="U13" s="48"/>
     </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="37"/>
       <c r="C14" s="36">
@@ -2610,7 +2619,7 @@
       <c r="T14" s="48"/>
       <c r="U14" s="48"/>
     </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="37"/>
       <c r="C15" s="36">
@@ -2653,7 +2662,7 @@
       <c r="T15" s="48"/>
       <c r="U15" s="48"/>
     </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="37"/>
       <c r="C16" s="36">
@@ -2696,7 +2705,7 @@
       <c r="T16" s="48"/>
       <c r="U16" s="48"/>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="37"/>
       <c r="C17" s="36">
@@ -2739,7 +2748,7 @@
       <c r="T17" s="48"/>
       <c r="U17" s="48"/>
     </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="37"/>
       <c r="C18" s="36">
@@ -2782,7 +2791,7 @@
       <c r="T18" s="48"/>
       <c r="U18" s="48"/>
     </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="37"/>
       <c r="C19" s="36">
@@ -2825,7 +2834,7 @@
       <c r="T19" s="48"/>
       <c r="U19" s="48"/>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="37"/>
       <c r="C20" s="36">
@@ -2868,7 +2877,7 @@
       <c r="T20" s="48"/>
       <c r="U20" s="48"/>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="37"/>
       <c r="C21" s="36">
@@ -2911,7 +2920,7 @@
       <c r="T21" s="48"/>
       <c r="U21" s="48"/>
     </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="37"/>
       <c r="C22" s="36">
@@ -2954,7 +2963,7 @@
       <c r="T22" s="48"/>
       <c r="U22" s="48"/>
     </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="37"/>
       <c r="C23" s="36">
@@ -2997,7 +3006,7 @@
       <c r="T23" s="48"/>
       <c r="U23" s="48"/>
     </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="37"/>
       <c r="C24" s="36">
@@ -3040,7 +3049,7 @@
       <c r="T24" s="48"/>
       <c r="U24" s="48"/>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="37"/>
       <c r="C25" s="36">
@@ -3083,7 +3092,7 @@
       <c r="T25" s="48"/>
       <c r="U25" s="48"/>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="37"/>
       <c r="C26" s="36">
@@ -3126,7 +3135,7 @@
       <c r="T26" s="48"/>
       <c r="U26" s="48"/>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="37"/>
       <c r="C27" s="36">
@@ -3169,7 +3178,7 @@
       <c r="T27" s="48"/>
       <c r="U27" s="48"/>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="37"/>
       <c r="C28" s="36">
@@ -3212,7 +3221,7 @@
       <c r="T28" s="48"/>
       <c r="U28" s="48"/>
     </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="37"/>
       <c r="C29" s="36">
@@ -3255,7 +3264,7 @@
       <c r="T29" s="48"/>
       <c r="U29" s="48"/>
     </row>
-    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="37"/>
       <c r="C30" s="36">
@@ -3298,27 +3307,27 @@
       <c r="T30" s="48"/>
       <c r="U30" s="48"/>
     </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C31" s="36">
         <v>0.5</v>
       </c>
       <c r="D31" s="38">
-        <f>SUM(D10:D30)</f>
-        <v>147</v>
+        <f>SUM(D10:D30)-7</f>
+        <v>140</v>
       </c>
       <c r="E31" s="38">
         <v>1</v>
       </c>
       <c r="F31" s="38">
-        <v>0.15</v>
+        <v>0.23</v>
       </c>
       <c r="G31" s="39">
         <f t="shared" si="3"/>
-        <v>11.025</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H31" s="40"/>
       <c r="I31" s="40"/>
@@ -3334,7 +3343,7 @@
       <c r="T31" s="48"/>
       <c r="U31" s="48"/>
     </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="37" t="s">
         <v>39</v>
@@ -3345,17 +3354,17 @@
       <c r="F32" s="38"/>
       <c r="G32" s="34">
         <f>SUM(G10:G31)</f>
-        <v>635.47197691252677</v>
+        <v>640.54697691252682</v>
       </c>
       <c r="H32" s="40" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="I32" s="40">
         <v>64.63</v>
       </c>
       <c r="J32" s="44">
         <f>G32*I32</f>
-        <v>41070.553867856601</v>
+        <v>41398.551117856608</v>
       </c>
       <c r="K32" s="21"/>
       <c r="N32" s="48"/>
@@ -3367,7 +3376,7 @@
       <c r="T32" s="48"/>
       <c r="U32" s="48"/>
     </row>
-    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="37" t="s">
         <v>38</v>
@@ -3381,11 +3390,11 @@
       <c r="I33" s="40"/>
       <c r="J33" s="44">
         <f>0.13*G32*19284/360</f>
-        <v>4425.2150232265321</v>
+        <v>4460.555631559866</v>
       </c>
       <c r="K33" s="21"/>
     </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
       <c r="B34" s="37"/>
       <c r="C34" s="42"/>
@@ -3398,7 +3407,7 @@
       <c r="J34" s="44"/>
       <c r="K34" s="36"/>
     </row>
-    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18">
         <v>2</v>
       </c>
@@ -3427,7 +3436,7 @@
       </c>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="24"/>
       <c r="C36" s="19"/>
@@ -3440,7 +3449,7 @@
       <c r="J36" s="41"/>
       <c r="K36" s="21"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
       <c r="B37" s="45" t="s">
         <v>17</v>
@@ -3454,11 +3463,11 @@
       <c r="I37" s="41"/>
       <c r="J37" s="41">
         <f>SUM(J9:J35)</f>
-        <v>45495.768891083135</v>
+        <v>45859.106749416474</v>
       </c>
       <c r="K37" s="36"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="57"/>
       <c r="B38" s="60"/>
       <c r="C38" s="61"/>
@@ -3471,16 +3480,16 @@
       <c r="J38" s="59"/>
       <c r="K38" s="56"/>
     </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49"/>
       <c r="B39" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="74">
+        <v>45</v>
+      </c>
+      <c r="C39" s="70">
         <f>J37</f>
-        <v>45495.768891083135</v>
-      </c>
-      <c r="D39" s="74"/>
+        <v>45859.106749416474</v>
+      </c>
+      <c r="D39" s="70"/>
       <c r="E39" s="51"/>
       <c r="F39" s="50"/>
       <c r="G39" s="51"/>
@@ -3489,15 +3498,15 @@
       <c r="J39" s="53"/>
       <c r="K39" s="54"/>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="55"/>
       <c r="B40" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="77">
+      <c r="C40" s="73">
         <v>40000</v>
       </c>
-      <c r="D40" s="77"/>
+      <c r="D40" s="73"/>
       <c r="E40" s="67"/>
       <c r="F40" s="48"/>
       <c r="G40" s="47"/>
@@ -3506,19 +3515,19 @@
       <c r="J40" s="47"/>
       <c r="K40" s="48"/>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="55"/>
       <c r="B41" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="78">
+      <c r="C41" s="74">
         <f>C40-C43-C44</f>
         <v>38000</v>
       </c>
-      <c r="D41" s="78"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="39">
         <f>C41/C39*100</f>
-        <v>83.524250553874566</v>
+        <v>82.862494918707768</v>
       </c>
       <c r="F41" s="48"/>
       <c r="G41" s="47"/>
@@ -3527,19 +3536,19 @@
       <c r="J41" s="47"/>
       <c r="K41" s="48"/>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="55"/>
       <c r="B42" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="74">
+      <c r="C42" s="70">
         <f>C39-C41</f>
-        <v>7495.7688910831348</v>
-      </c>
-      <c r="D42" s="74"/>
+        <v>7859.1067494164745</v>
+      </c>
+      <c r="D42" s="70"/>
       <c r="E42" s="39">
         <f>100-E41</f>
-        <v>16.475749446125434</v>
+        <v>17.137505081292232</v>
       </c>
       <c r="F42" s="48"/>
       <c r="G42" s="47"/>
@@ -3548,16 +3557,16 @@
       <c r="J42" s="47"/>
       <c r="K42" s="48"/>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="55"/>
       <c r="B43" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="74">
+      <c r="C43" s="70">
         <f>C40*0.03</f>
         <v>1200</v>
       </c>
-      <c r="D43" s="74"/>
+      <c r="D43" s="70"/>
       <c r="E43" s="39">
         <v>3</v>
       </c>
@@ -3568,16 +3577,16 @@
       <c r="J43" s="47"/>
       <c r="K43" s="48"/>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="55"/>
       <c r="B44" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="74">
+      <c r="C44" s="70">
         <f>C40*0.02</f>
         <v>800</v>
       </c>
-      <c r="D44" s="74"/>
+      <c r="D44" s="70"/>
       <c r="E44" s="39">
         <v>2</v>
       </c>
@@ -3588,7 +3597,7 @@
       <c r="J44" s="47"/>
       <c r="K44" s="48"/>
     </row>
-    <row r="45" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="56"/>
       <c r="B45" s="56"/>
       <c r="C45" s="56"/>
@@ -3601,57 +3610,64 @@
       <c r="J45" s="56"/>
       <c r="K45" s="56"/>
     </row>
-    <row r="46" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="A7:F7"/>
@@ -3660,21 +3676,1480 @@
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+    </row>
+    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+    </row>
+    <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+    </row>
+    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="2"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="93"/>
+      <c r="K6" s="68" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="3"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="69" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>1</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="21"/>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="64">
+        <v>4</v>
+      </c>
+      <c r="O9">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="38">
+        <f>M10</f>
+        <v>7</v>
+      </c>
+      <c r="E10" s="38">
+        <f>(N9+N10)/2</f>
+        <v>4.5</v>
+      </c>
+      <c r="F10" s="38">
+        <f>(O9+O10)/2</f>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="G10" s="39">
+        <f>PRODUCT(C10:F10)</f>
+        <v>12.993749999999999</v>
+      </c>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="21"/>
+      <c r="M10" s="48">
+        <v>7</v>
+      </c>
+      <c r="N10" s="65">
+        <v>5</v>
+      </c>
+      <c r="O10" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="38">
+        <f t="shared" ref="D11:D30" si="0">M11</f>
+        <v>7</v>
+      </c>
+      <c r="E11" s="38">
+        <f t="shared" ref="E11:F30" si="1">(N10+N11)/2</f>
+        <v>5.5</v>
+      </c>
+      <c r="F11" s="38">
+        <f t="shared" si="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="G11" s="39">
+        <f t="shared" ref="G11:G31" si="2">PRODUCT(C11:F11)</f>
+        <v>35.612500000000004</v>
+      </c>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="21"/>
+      <c r="M11" s="48">
+        <v>7</v>
+      </c>
+      <c r="N11" s="65">
+        <v>6</v>
+      </c>
+      <c r="O11" s="48">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E12" s="38">
+        <f t="shared" si="1"/>
+        <v>4.8287107589149647</v>
+      </c>
+      <c r="F12" s="38">
+        <f t="shared" si="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="G12" s="39">
+        <f t="shared" si="2"/>
+        <v>31.265902163974395</v>
+      </c>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="21"/>
+      <c r="M12" s="48">
+        <v>7</v>
+      </c>
+      <c r="N12" s="65">
+        <f>12/3.281</f>
+        <v>3.6574215178299299</v>
+      </c>
+      <c r="O12" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E13" s="38">
+        <f t="shared" si="1"/>
+        <v>3.6574215178299299</v>
+      </c>
+      <c r="F13" s="38">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="G13" s="39">
+        <f t="shared" si="2"/>
+        <v>19.201462968607132</v>
+      </c>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="21"/>
+      <c r="M13" s="48">
+        <v>7</v>
+      </c>
+      <c r="N13" s="65">
+        <f>12/3.281</f>
+        <v>3.6574215178299299</v>
+      </c>
+      <c r="O13" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E14" s="38">
+        <f t="shared" si="1"/>
+        <v>4.1145992075586708</v>
+      </c>
+      <c r="F14" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G14" s="39">
+        <f t="shared" si="2"/>
+        <v>28.802194452910697</v>
+      </c>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="21"/>
+      <c r="M14" s="48">
+        <v>7</v>
+      </c>
+      <c r="N14" s="65">
+        <f>15/3.281</f>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O14" s="48">
+        <v>2.5</v>
+      </c>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="48"/>
+      <c r="U14" s="48"/>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E15" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F15" s="38">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="G15" s="39">
+        <f t="shared" si="2"/>
+        <v>36.002743066138372</v>
+      </c>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="21"/>
+      <c r="M15" s="48">
+        <v>7</v>
+      </c>
+      <c r="N15" s="65">
+        <f t="shared" ref="N15:N30" si="3">15/3.281</f>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O15" s="48">
+        <v>2</v>
+      </c>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="48"/>
+      <c r="R15" s="48"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="48"/>
+      <c r="U15" s="48"/>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E16" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F16" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G16" s="39">
+        <f t="shared" si="2"/>
+        <v>32.002438281011884</v>
+      </c>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="21"/>
+      <c r="M16" s="48">
+        <v>7</v>
+      </c>
+      <c r="N16" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O16" s="48">
+        <v>2</v>
+      </c>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="48"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="48"/>
+      <c r="U16" s="48"/>
+    </row>
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E17" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F17" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G17" s="39">
+        <f t="shared" si="2"/>
+        <v>32.002438281011884</v>
+      </c>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="21"/>
+      <c r="M17" s="48">
+        <v>7</v>
+      </c>
+      <c r="N17" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O17" s="48">
+        <v>2</v>
+      </c>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
+      <c r="R17" s="48"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+    </row>
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E18" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F18" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G18" s="39">
+        <f t="shared" si="2"/>
+        <v>32.002438281011884</v>
+      </c>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="21"/>
+      <c r="M18" s="48">
+        <v>7</v>
+      </c>
+      <c r="N18" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O18" s="48">
+        <v>2</v>
+      </c>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+    </row>
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E19" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F19" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G19" s="39">
+        <f t="shared" si="2"/>
+        <v>32.002438281011884</v>
+      </c>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="21"/>
+      <c r="M19" s="48">
+        <v>7</v>
+      </c>
+      <c r="N19" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O19" s="48">
+        <v>2</v>
+      </c>
+      <c r="P19" s="48"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="48"/>
+      <c r="S19" s="48"/>
+      <c r="T19" s="48"/>
+      <c r="U19" s="48"/>
+    </row>
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E20" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F20" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G20" s="39">
+        <f t="shared" si="2"/>
+        <v>32.002438281011884</v>
+      </c>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="21"/>
+      <c r="M20" s="48">
+        <v>7</v>
+      </c>
+      <c r="N20" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O20" s="48">
+        <v>2</v>
+      </c>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+    </row>
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E21" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F21" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G21" s="39">
+        <f t="shared" si="2"/>
+        <v>32.002438281011884</v>
+      </c>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="21"/>
+      <c r="M21" s="48">
+        <v>7</v>
+      </c>
+      <c r="N21" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O21" s="48">
+        <v>2</v>
+      </c>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
+    </row>
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E22" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F22" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G22" s="39">
+        <f t="shared" si="2"/>
+        <v>32.002438281011884</v>
+      </c>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="21"/>
+      <c r="M22" s="48">
+        <v>7</v>
+      </c>
+      <c r="N22" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O22" s="48">
+        <v>2</v>
+      </c>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
+    </row>
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E23" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F23" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G23" s="39">
+        <f t="shared" si="2"/>
+        <v>32.002438281011884</v>
+      </c>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="21"/>
+      <c r="M23" s="48">
+        <v>7</v>
+      </c>
+      <c r="N23" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O23" s="48">
+        <v>2</v>
+      </c>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="48"/>
+      <c r="U23" s="48"/>
+    </row>
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E24" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F24" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G24" s="39">
+        <f t="shared" si="2"/>
+        <v>32.002438281011884</v>
+      </c>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="21"/>
+      <c r="M24" s="48">
+        <v>7</v>
+      </c>
+      <c r="N24" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O24" s="48">
+        <v>2</v>
+      </c>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48"/>
+      <c r="U24" s="48"/>
+    </row>
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E25" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F25" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G25" s="39">
+        <f t="shared" si="2"/>
+        <v>32.002438281011884</v>
+      </c>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="21"/>
+      <c r="M25" s="48">
+        <v>7</v>
+      </c>
+      <c r="N25" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O25" s="48">
+        <v>2</v>
+      </c>
+      <c r="P25" s="48"/>
+      <c r="Q25" s="48"/>
+      <c r="R25" s="48"/>
+      <c r="S25" s="48"/>
+      <c r="T25" s="48"/>
+      <c r="U25" s="48"/>
+    </row>
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E26" s="38">
+        <f t="shared" si="1"/>
+        <v>5.3337397135019806</v>
+      </c>
+      <c r="F26" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G26" s="39">
+        <f t="shared" si="2"/>
+        <v>37.336177994513861</v>
+      </c>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="21"/>
+      <c r="M26" s="48">
+        <v>7</v>
+      </c>
+      <c r="N26" s="65">
+        <f>20/3.281</f>
+        <v>6.0957025297165499</v>
+      </c>
+      <c r="O26" s="48">
+        <v>2</v>
+      </c>
+      <c r="P26" s="48"/>
+      <c r="Q26" s="48"/>
+      <c r="R26" s="48"/>
+      <c r="S26" s="48"/>
+      <c r="T26" s="48"/>
+      <c r="U26" s="48"/>
+    </row>
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E27" s="38">
+        <f t="shared" si="1"/>
+        <v>6.0957025297165499</v>
+      </c>
+      <c r="F27" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G27" s="39">
+        <f t="shared" si="2"/>
+        <v>42.669917708015852</v>
+      </c>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="21"/>
+      <c r="M27" s="1">
+        <v>7</v>
+      </c>
+      <c r="N27" s="65">
+        <f>20/3.281</f>
+        <v>6.0957025297165499</v>
+      </c>
+      <c r="O27" s="48">
+        <v>2</v>
+      </c>
+      <c r="P27" s="48"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="48"/>
+      <c r="S27" s="48"/>
+      <c r="T27" s="48"/>
+      <c r="U27" s="48"/>
+    </row>
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E28" s="38">
+        <f t="shared" si="1"/>
+        <v>5.3337397135019806</v>
+      </c>
+      <c r="F28" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G28" s="39">
+        <f t="shared" si="2"/>
+        <v>37.336177994513861</v>
+      </c>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="21"/>
+      <c r="M28" s="48">
+        <v>7</v>
+      </c>
+      <c r="N28" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O28" s="48">
+        <v>2</v>
+      </c>
+      <c r="P28" s="48"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="48"/>
+      <c r="T28" s="48"/>
+      <c r="U28" s="48"/>
+    </row>
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E29" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F29" s="38">
+        <f t="shared" si="1"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G29" s="39">
+        <f t="shared" si="2"/>
+        <v>18.401402011581833</v>
+      </c>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="21"/>
+      <c r="M29" s="48">
+        <v>7</v>
+      </c>
+      <c r="N29" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O29" s="48">
+        <v>0.3</v>
+      </c>
+      <c r="P29" s="48"/>
+      <c r="Q29" s="48"/>
+      <c r="R29" s="48"/>
+      <c r="S29" s="48"/>
+      <c r="T29" s="48"/>
+      <c r="U29" s="48"/>
+    </row>
+    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E30" s="38">
+        <f t="shared" si="1"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F30" s="38">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="G30" s="39">
+        <f t="shared" si="2"/>
+        <v>4.800365742151782</v>
+      </c>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="21"/>
+      <c r="M30" s="48">
+        <v>7</v>
+      </c>
+      <c r="N30" s="65">
+        <f t="shared" si="3"/>
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="O30" s="48">
+        <v>0.3</v>
+      </c>
+      <c r="P30" s="48"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="48"/>
+      <c r="S30" s="48"/>
+      <c r="T30" s="48"/>
+      <c r="U30" s="48"/>
+    </row>
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="38">
+        <f>SUM(D10:D30)-7</f>
+        <v>140</v>
+      </c>
+      <c r="E31" s="38">
+        <v>1</v>
+      </c>
+      <c r="F31" s="38">
+        <v>0.23</v>
+      </c>
+      <c r="G31" s="39">
+        <f t="shared" si="2"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="21"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="65"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48"/>
+      <c r="T31" s="48"/>
+      <c r="U31" s="48"/>
+    </row>
+    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="36"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="34">
+        <f>SUM(G10:G31)</f>
+        <v>640.54697691252682</v>
+      </c>
+      <c r="H32" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="I32" s="40">
+        <v>64.63</v>
+      </c>
+      <c r="J32" s="44">
+        <f>G32*I32</f>
+        <v>41398.551117856608</v>
+      </c>
+      <c r="K32" s="21"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="48"/>
+      <c r="P32" s="48"/>
+      <c r="Q32" s="48"/>
+      <c r="R32" s="48"/>
+      <c r="S32" s="48"/>
+      <c r="T32" s="48"/>
+      <c r="U32" s="48"/>
+    </row>
+    <row r="33" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="36"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="44">
+        <f>0.13*G32*19284/360</f>
+        <v>4460.555631559866</v>
+      </c>
+      <c r="K33" s="21"/>
+    </row>
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="40"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="36"/>
+    </row>
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <v>2</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="19">
+        <v>0</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="34">
+        <f t="shared" ref="G35" si="4">PRODUCT(C35:F35)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="23">
+        <v>500</v>
+      </c>
+      <c r="J35" s="34">
+        <f>G35*I35</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="21"/>
+    </row>
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="21"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="40"/>
+      <c r="B37" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="46"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41">
+        <f>SUM(J9:J35)</f>
+        <v>45859.106749416474</v>
+      </c>
+      <c r="K37" s="36"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="57"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="59"/>
+      <c r="J38" s="59"/>
+      <c r="K38" s="56"/>
+    </row>
+    <row r="39" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="49"/>
+      <c r="B39" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="70">
+        <f>J37</f>
+        <v>45859.106749416474</v>
+      </c>
+      <c r="D39" s="70"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="54"/>
+    </row>
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="55"/>
+      <c r="B40" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="73">
+        <v>40000</v>
+      </c>
+      <c r="D40" s="73"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="48"/>
+    </row>
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="55"/>
+      <c r="B41" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="74">
+        <f>C40-C43-C44</f>
+        <v>38000</v>
+      </c>
+      <c r="D41" s="74"/>
+      <c r="E41" s="39">
+        <f>C41/C39*100</f>
+        <v>82.862494918707768</v>
+      </c>
+      <c r="F41" s="48"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="48"/>
+    </row>
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="55"/>
+      <c r="B42" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="70">
+        <f>C39-C41</f>
+        <v>7859.1067494164745</v>
+      </c>
+      <c r="D42" s="70"/>
+      <c r="E42" s="39">
+        <f>100-E41</f>
+        <v>17.137505081292232</v>
+      </c>
+      <c r="F42" s="48"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="48"/>
+    </row>
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="55"/>
+      <c r="B43" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="70">
+        <f>C40*0.03</f>
+        <v>1200</v>
+      </c>
+      <c r="D43" s="70"/>
+      <c r="E43" s="39">
+        <v>3</v>
+      </c>
+      <c r="F43" s="48"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="48"/>
+    </row>
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="55"/>
+      <c r="B44" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="70">
+        <f>C40*0.02</f>
+        <v>800</v>
+      </c>
+      <c r="D44" s="70"/>
+      <c r="E44" s="39">
+        <v>2</v>
+      </c>
+      <c r="F44" s="48"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="48"/>
+    </row>
+    <row r="45" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="56"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+    </row>
+    <row r="46" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;LPrepared By:
-Kristal Suwal&amp;CChecked By:
-Er. Milan Phuyal&amp;RApproved By:
-Er. Prakash Singh Saud</oddFooter>
+    <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>